<commit_message>
Finish check_plot_inputs and prep_config w accessories and tests
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E052A4-110C-4026-8A5E-EE54B69CE263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F50C6E6-4ED7-4546-AB76-19D8C749763F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="5" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="8" activeTab="20" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,20 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
+    <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
+    <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="60">
   <si>
     <t>stacked</t>
   </si>
@@ -126,6 +140,102 @@
   </si>
   <si>
     <t>SURS--0300230S--P31_S14sdf_D--G4--N--Q</t>
+  </si>
+  <si>
+    <t>velikost</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>število</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>10,20,30</t>
+  </si>
+  <si>
+    <t>Serija 2</t>
+  </si>
+  <si>
+    <t>stolpec</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>Serija 3</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P31_S13_D--G4--N--Q</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P31_S23_D--G4--N--Q</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>desna</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>medletna</t>
+  </si>
+  <si>
+    <t>QOQ</t>
+  </si>
+  <si>
+    <t>MOM</t>
+  </si>
+  <si>
+    <t>YOY</t>
+  </si>
+  <si>
+    <t>2015Q1</t>
+  </si>
+  <si>
+    <t>2015M02</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>Serija 4</t>
+  </si>
+  <si>
+    <t>SURS--030030S--P31_S14_D--G4--N--M</t>
+  </si>
+  <si>
+    <t>SURS--0330S--P31_S15_D--G4--N--A</t>
+  </si>
+  <si>
+    <t>SURS--0330S--P31_S13_D--G4--N--A</t>
+  </si>
+  <si>
+    <t>SURS--030S--P31_S_D--G4--N--A</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P31_S1ss3_D--G4--N--Q</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -479,15 +589,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80EE0B4-0DE5-4420-9F2D-2330D5CD04DC}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -519,36 +629,1965 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB519D6D-497D-4A71-AA43-35FF7CBDA7D6}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C50B29-7A1F-44EC-A2E3-6FFB5D7AF5C3}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D794E32-1D66-4AE3-9459-DCC88E8958D7}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C3197-EE10-4F45-AA72-93BAA0310B66}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J5" sqref="J2:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A0D24B-06B1-46C1-B24E-D0229212BA8F}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384968AD-14AF-4C49-8E39-1D8EB64036E4}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5A0802-79CF-41E4-9C0C-B7CF9AB66D55}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF6D7A-E8BF-4A5F-92E8-83A3842A5065}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A051C55C-5114-4B50-9EEA-9971CA4766EF}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6814E3-30B1-4C15-9D30-846626E50BDB}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -558,15 +2597,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDA8BA5-AD9E-45CA-A388-27BBF83C10CE}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -598,31 +2637,34 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -638,14 +2680,628 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67294519-493C-4162-90F2-F70A28CBB2F0}">
+  <dimension ref="A1:S8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2">
+        <v>2015</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+      <c r="O7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N8">
+        <v>12</v>
+      </c>
+      <c r="O8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C29FF1A-9024-4DF3-916F-A0BDB0709BF3}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -655,15 +3311,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A43C6C-A966-4635-89A5-EACCD8BF4906}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -695,31 +3351,34 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -735,17 +3394,17 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -761,13 +3420,13 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3">
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
     </row>
@@ -778,15 +3437,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -818,31 +3477,34 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -858,20 +3520,20 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1">
-        <v>36557</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -887,16 +3549,16 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
         <v>36617</v>
       </c>
-      <c r="N3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3">
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
     </row>
@@ -907,15 +3569,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209DCC60-78F8-43ED-886D-BA241054DEC9}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -947,31 +3609,34 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -987,32 +3652,32 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1">
-        <v>36557</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
         <v>123</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1028,28 +3693,28 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>36617</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>13</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>24</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
       <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>2</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>321</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>123</v>
       </c>
     </row>
@@ -1060,15 +3725,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027D9544-C268-4861-A247-C7F1D198DA75}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1100,31 +3765,34 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1137,40 +3805,40 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1">
-        <v>36557</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2">
-        <v>12</v>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
         <v>123</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -1178,28 +3846,28 @@
       <c r="J3">
         <v>2015</v>
       </c>
-      <c r="K3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="1">
-        <v>36557</v>
-      </c>
-      <c r="M3">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3">
-        <v>12</v>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>123</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>321</v>
       </c>
     </row>
@@ -1210,15 +3878,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415E4898-F92C-452A-84DB-D5677E1E5900}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1250,31 +3918,34 @@
         <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1290,20 +3961,26 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1">
-        <v>36557</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1319,7 +3996,360 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="P3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7E6D6-EE7B-468F-B872-C3BE058F00D0}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E2F05C-93A5-44D7-9D90-57CE56FE1A56}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2015</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add get_data and update dates funs with tests and mocks
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F50C6E6-4ED7-4546-AB76-19D8C749763F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7EABA4-8B39-44E8-8075-8C7BD4590F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="8" activeTab="20" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="11" activeTab="21" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
     <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
     <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
+    <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="68">
   <si>
     <t>stacked</t>
   </si>
@@ -236,6 +237,30 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>MF--OB--001--7--A</t>
+  </si>
+  <si>
+    <t>SKUPAJ PRIHODKI -- Letno</t>
+  </si>
+  <si>
+    <t>eur</t>
+  </si>
+  <si>
+    <t>MF--OB--001--7--M</t>
+  </si>
+  <si>
+    <t>SKUPAJ PRIHODKI -- Mesečno</t>
+  </si>
+  <si>
+    <t>19 Proizvodnja koksa in naftnih derivatov -- Podjetja v % -- negotove gospodarske razmere</t>
+  </si>
+  <si>
+    <t>-100, 0, 100</t>
+  </si>
+  <si>
+    <t>0, 50000, 100000</t>
   </si>
 </sst>
 </file>
@@ -272,9 +297,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,7 +700,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3072,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C29FF1A-9024-4DF3-916F-A0BDB0709BF3}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,6 +3328,119 @@
       </c>
       <c r="P5">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F90AD-04CA-45FB-9D9A-2BBE8BFC6DB7}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4">
+        <v>2015</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add transformation funs with accessories
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7EABA4-8B39-44E8-8075-8C7BD4590F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693922BC-B3AC-4B40-967B-C95685958FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="11" activeTab="21" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="12" activeTab="23" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,8 @@
     <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
     <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
     <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
+    <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
+    <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="70">
   <si>
     <t>stacked</t>
   </si>
@@ -261,6 +263,12 @@
   </si>
   <si>
     <t>0, 50000, 100000</t>
+  </si>
+  <si>
+    <t>qoq</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P31_S14_D--G4--N--M</t>
   </si>
 </sst>
 </file>
@@ -3099,7 +3107,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3339,7 +3347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F90AD-04CA-45FB-9D9A-2BBE8BFC6DB7}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3441,6 +3449,333 @@
       </c>
       <c r="S4" t="s">
         <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184719B6-2593-48D2-ACDD-B538913534C8}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="A1:S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2">
+        <v>2015</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA275B0-0109-45DF-8346-6D8E9FCBBD4F}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data prep and transform pipeline for publ.ready charts done. w tests
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693922BC-B3AC-4B40-967B-C95685958FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEA3F64-EFB4-4441-83E5-A0CE0824CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="12" activeTab="23" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView minimized="1" xWindow="1515" yWindow="1515" windowWidth="18900" windowHeight="11160" firstSheet="17" activeTab="24" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
     <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
     <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
+    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="73">
   <si>
     <t>stacked</t>
   </si>
@@ -269,6 +270,15 @@
   </si>
   <si>
     <t>SURS--0300230S--P31_S14_D--G4--N--M</t>
+  </si>
+  <si>
+    <t>Indeks</t>
+  </si>
+  <si>
+    <t>SURS--0427601S--H53--6--Q</t>
+  </si>
+  <si>
+    <t>indeks</t>
   </si>
 </sst>
 </file>
@@ -3348,7 +3358,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,16 +3432,22 @@
       <c r="C2" t="s">
         <v>61</v>
       </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -3461,7 +3477,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="A1:S3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA275B0-0109-45DF-8346-6D8E9FCBBD4F}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3776,6 +3792,91 @@
       </c>
       <c r="P3">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2">
+        <v>2010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start on publ ready plots w tests and mocks
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEA3F64-EFB4-4441-83E5-A0CE0824CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF0BA2B-E426-476E-BD62-716EA936EA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1515" yWindow="1515" windowWidth="18900" windowHeight="11160" firstSheet="17" activeTab="24" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="4080" yWindow="3930" windowWidth="18900" windowHeight="11160" firstSheet="19" activeTab="24" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,9 @@
     <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
     <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
     <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
-    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheet26" sheetId="26" r:id="rId25"/>
+    <sheet name="Sheet25" sheetId="25" r:id="rId26"/>
+    <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="74">
   <si>
     <t>stacked</t>
   </si>
@@ -212,12 +214,6 @@
     <t>YOY</t>
   </si>
   <si>
-    <t>2015Q1</t>
-  </si>
-  <si>
-    <t>2015M02</t>
-  </si>
-  <si>
     <t>sdf</t>
   </si>
   <si>
@@ -272,13 +268,22 @@
     <t>SURS--0300230S--P31_S14_D--G4--N--M</t>
   </si>
   <si>
-    <t>Indeks</t>
-  </si>
-  <si>
     <t>SURS--0427601S--H53--6--Q</t>
   </si>
   <si>
     <t>indeks</t>
+  </si>
+  <si>
+    <t>SURS--0427601S--H53.1--1--Q</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C3197-EE10-4F45-AA72-93BAA0310B66}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
@@ -1835,7 +1840,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,7 +1921,7 @@
         <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
         <v>46</v>
@@ -1966,7 +1971,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2004,7 +2009,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -2034,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF6D7A-E8BF-4A5F-92E8-83A3842A5065}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
@@ -2744,7 +2749,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J6" sqref="J6:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,8 +2879,8 @@
       <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
-        <v>50</v>
+      <c r="J3">
+        <v>2015</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2915,8 +2920,8 @@
       <c r="H4" t="s">
         <v>45</v>
       </c>
-      <c r="J4" t="s">
-        <v>51</v>
+      <c r="J4">
+        <v>2015</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -2939,13 +2944,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -2957,7 +2962,7 @@
         <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -2986,7 +2991,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -3006,8 +3011,8 @@
       <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
-        <v>50</v>
+      <c r="J6">
+        <v>2015</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -3030,7 +3035,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -3047,8 +3052,8 @@
       <c r="H7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" t="s">
-        <v>51</v>
+      <c r="J7">
+        <v>2015</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -3071,7 +3076,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -3087,6 +3092,9 @@
       </c>
       <c r="H8" t="s">
         <v>45</v>
+      </c>
+      <c r="J8">
+        <v>2015</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -3117,7 +3125,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="N3" sqref="N3:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,8 +3220,8 @@
       <c r="M2" s="1">
         <v>36557</v>
       </c>
-      <c r="N2">
-        <v>12</v>
+      <c r="N2" s="1">
+        <v>44621</v>
       </c>
       <c r="O2" t="s">
         <v>8</v>
@@ -3259,8 +3267,8 @@
       <c r="M3" s="1">
         <v>36557</v>
       </c>
-      <c r="N3">
-        <v>12</v>
+      <c r="N3" s="1">
+        <v>44621</v>
       </c>
       <c r="O3" t="s">
         <v>8</v>
@@ -3300,8 +3308,8 @@
       <c r="M4" s="1">
         <v>36557</v>
       </c>
-      <c r="N4">
-        <v>12</v>
+      <c r="N4" s="1">
+        <v>44621</v>
       </c>
       <c r="O4" t="s">
         <v>8</v>
@@ -3312,13 +3320,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -3338,8 +3346,8 @@
       <c r="M5" s="1">
         <v>36557</v>
       </c>
-      <c r="N5">
-        <v>12</v>
+      <c r="N5" s="1">
+        <v>44621</v>
       </c>
       <c r="O5" t="s">
         <v>8</v>
@@ -3358,7 +3366,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3424,13 +3432,13 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I2" t="s">
         <v>49</v>
@@ -3438,13 +3446,13 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -3455,16 +3463,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J4">
         <v>2015</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3642,7 +3650,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,7 +3716,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3726,7 +3734,7 @@
         <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -3800,10 +3808,157 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2" s="1">
+        <v>37316</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3" s="1">
+        <v>37316</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3870,13 +4025,169 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J2">
         <v>2010</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6187-8CFA-4331-9ECF-E1D00B50A721}">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36891</v>
+      </c>
+      <c r="N2" s="1">
+        <v>36220</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36891</v>
+      </c>
+      <c r="N3" s="1">
+        <v>36220</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4303,7 +4614,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N2" sqref="N2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,9 +4697,6 @@
       <c r="M2" s="1">
         <v>36557</v>
       </c>
-      <c r="N2">
-        <v>12</v>
-      </c>
       <c r="O2" t="s">
         <v>8</v>
       </c>
@@ -4426,9 +4734,6 @@
       </c>
       <c r="M3" s="1">
         <v>36557</v>
-      </c>
-      <c r="N3">
-        <v>12</v>
       </c>
       <c r="O3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
PUbl. ready charts titles, legends, left yaxis, bars and some line stuff :fire: :sparkles: :fire:
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF0BA2B-E426-476E-BD62-716EA936EA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CAD547-E030-413A-BD5D-3C847C4D0933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="3930" windowWidth="18900" windowHeight="11160" firstSheet="19" activeTab="24" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="19" activeTab="29" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,10 @@
     <sheet name="Sheet26" sheetId="26" r:id="rId25"/>
     <sheet name="Sheet25" sheetId="25" r:id="rId26"/>
     <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
+    <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
+    <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
+    <sheet name="Sheet31" sheetId="31" r:id="rId30"/>
+    <sheet name="Sheet30" sheetId="30" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="99">
   <si>
     <t>stacked</t>
   </si>
@@ -284,6 +288,81 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>SURS--0457101S--C28--07--M</t>
+  </si>
+  <si>
+    <t>SURS--0457101S--C28--11--M</t>
+  </si>
+  <si>
+    <t>Serija 1 malo daljša</t>
+  </si>
+  <si>
+    <t>Serija 3 še daljša kot enka</t>
+  </si>
+  <si>
+    <t>SURS--0457101S--C29--01--M</t>
+  </si>
+  <si>
+    <t>Serija 5</t>
+  </si>
+  <si>
+    <t>MF--DP--001--7--A</t>
+  </si>
+  <si>
+    <t>MF--DP--002--901--A</t>
+  </si>
+  <si>
+    <t>enka</t>
+  </si>
+  <si>
+    <t>dvojka</t>
+  </si>
+  <si>
+    <t>MF--DP--003--70--A</t>
+  </si>
+  <si>
+    <t>trojka</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--B1GQ--G4--N--Q</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P3_S13--GO4--N--Q</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P31_S14_D--GO4--N--Q</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P51G--GO4--N--Q</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--P52--GO4--N--Q</t>
+  </si>
+  <si>
+    <t>SURS--0300230S--B11--GO4--N--Q</t>
+  </si>
+  <si>
+    <t>odstotne točke</t>
+  </si>
+  <si>
+    <t>Bruto domači proizvod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">....Končna potrošnja države </t>
+  </si>
+  <si>
+    <t>....Končna potrošnja gospodinjstev</t>
+  </si>
+  <si>
+    <t>....Bruto investicije v osnovna sredstva</t>
+  </si>
+  <si>
+    <t>....Spremembe zalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo menjave s tujino </t>
   </si>
 </sst>
 </file>
@@ -3811,7 +3890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4044,7 +4123,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4188,6 +4267,373 @@
       </c>
       <c r="P3">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324E071-F609-4FB8-B88D-8F0EE9A8EC4A}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43465</v>
+      </c>
+      <c r="N2" s="1">
+        <v>43891</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43465</v>
+      </c>
+      <c r="N3" s="1">
+        <v>43891</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4B2C62-126F-422E-B778-C7A7EC6134D3}">
+  <dimension ref="A1:S6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43465</v>
+      </c>
+      <c r="N2" s="1">
+        <v>43891</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1">
+        <v>43465</v>
+      </c>
+      <c r="N5" s="1">
+        <v>43891</v>
+      </c>
+      <c r="O5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4321,6 +4767,304 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C665D4F1-6FFE-4D8B-A6C9-DB93740290E1}">
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40909</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40179</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
   <dimension ref="A1:S3"/>

</xml_diff>

<commit_message>
Add margin and axis label funs and line drawing for pub ready charts
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CAD547-E030-413A-BD5D-3C847C4D0933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132CFB38-B98C-44CF-8E62-98D279FA3B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="19" activeTab="29" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="21" activeTab="31" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,8 +42,9 @@
     <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
     <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
     <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
-    <sheet name="Sheet31" sheetId="31" r:id="rId30"/>
-    <sheet name="Sheet30" sheetId="30" r:id="rId31"/>
+    <sheet name="Sheet30" sheetId="30" r:id="rId30"/>
+    <sheet name="Sheet31" sheetId="31" r:id="rId31"/>
+    <sheet name="Sheet32" sheetId="32" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="99">
   <si>
     <t>stacked</t>
   </si>
@@ -4768,11 +4769,124 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40179</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C665D4F1-6FFE-4D8B-A6C9-DB93740290E1}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="A1:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4952,12 +5066,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
-  <dimension ref="A1:S4"/>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54082569-1F66-4A81-82A5-55EB02F2FDFA}">
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,41 +5137,92 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1">
-        <v>40179</v>
+        <v>40909</v>
       </c>
       <c r="N2" s="1">
-        <v>44927</v>
+        <v>45292</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add x_sub_annual to config
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132CFB38-B98C-44CF-8E62-98D279FA3B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32DC63B-C0B5-4D47-A238-5EFEF6615979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="21" activeTab="31" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="100">
   <si>
     <t>stacked</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t xml:space="preserve">Saldo menjave s tujino </t>
+  </si>
+  <si>
+    <t>x_brez_let</t>
   </si>
 </sst>
 </file>
@@ -718,15 +721,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80EE0B4-0DE5-4420-9F2D-2330D5CD04DC}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -784,8 +787,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -800,15 +806,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB519D6D-497D-4A71-AA43-35FF7CBDA7D6}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -866,8 +872,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -911,7 +920,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -956,15 +965,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C50B29-7A1F-44EC-A2E3-6FFB5D7AF5C3}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J3"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1022,8 +1031,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1067,7 +1079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1112,15 +1124,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D794E32-1D66-4AE3-9459-DCC88E8958D7}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1178,8 +1190,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1258,7 +1273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1303,15 +1318,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C3197-EE10-4F45-AA72-93BAA0310B66}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J2:J5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1369,8 +1384,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1411,7 +1429,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1449,7 +1467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1484,7 +1502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1529,15 +1547,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A0D24B-06B1-46C1-B24E-D0229212BA8F}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1595,8 +1613,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1640,7 +1661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1681,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1726,15 +1747,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384968AD-14AF-4C49-8E39-1D8EB64036E4}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1792,8 +1813,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +1861,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1875,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1917,15 +1941,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5A0802-79CF-41E4-9C0C-B7CF9AB66D55}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1983,8 +2007,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2031,7 +2058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2072,7 +2099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2117,15 +2144,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF6D7A-E8BF-4A5F-92E8-83A3842A5065}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2183,8 +2210,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2231,7 +2261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2272,7 +2302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2317,15 +2347,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A051C55C-5114-4B50-9EEA-9971CA4766EF}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:S4"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2383,8 +2413,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2428,7 +2461,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2469,7 +2502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2514,15 +2547,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6814E3-30B1-4C15-9D30-846626E50BDB}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2580,8 +2613,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2628,7 +2664,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2675,7 +2711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2726,15 +2762,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDA8BA5-AD9E-45CA-A388-27BBF83C10CE}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2792,8 +2828,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2826,15 +2865,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67294519-493C-4162-90F2-F70A28CBB2F0}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J8"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2892,8 +2931,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2940,7 +2982,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2981,7 +3023,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3022,7 +3064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3069,7 +3111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3113,7 +3155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -3154,7 +3196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -3202,15 +3244,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C29FF1A-9024-4DF3-916F-A0BDB0709BF3}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3268,8 +3310,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3316,7 +3361,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3357,7 +3402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3398,7 +3443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3443,15 +3488,15 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F90AD-04CA-45FB-9D9A-2BBE8BFC6DB7}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3509,8 +3554,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -3524,7 +3572,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -3538,7 +3586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3562,15 +3610,15 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184719B6-2593-48D2-ACDD-B538913534C8}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3628,8 +3676,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3679,7 +3730,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3727,15 +3778,15 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA275B0-0109-45DF-8346-6D8E9FCBBD4F}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3793,8 +3844,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -3841,7 +3895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3889,15 +3943,15 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3955,8 +4009,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -3991,7 +4048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4036,15 +4093,15 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4102,8 +4159,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4121,10 +4181,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6187-8CFA-4331-9ECF-E1D00B50A721}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,7 +4192,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4190,8 +4250,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4229,7 +4292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4277,10 +4340,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324E071-F609-4FB8-B88D-8F0EE9A8EC4A}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4351,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4346,8 +4409,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4385,7 +4451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4426,7 +4492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4437,7 +4503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -4455,10 +4521,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4B2C62-126F-422E-B778-C7A7EC6134D3}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4466,7 +4532,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4524,8 +4590,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4566,7 +4635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -4577,7 +4646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -4588,7 +4657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4626,7 +4695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -4644,15 +4713,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A43C6C-A966-4635-89A5-EACCD8BF4906}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4710,8 +4779,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4737,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4770,15 +4842,15 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4836,8 +4908,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -4854,7 +4929,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -4865,7 +4940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4883,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C665D4F1-6FFE-4D8B-A6C9-DB93740290E1}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="A1:S7"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4894,7 +4969,7 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4952,8 +5027,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -4976,7 +5054,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -4993,7 +5071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5010,7 +5088,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5027,7 +5105,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5044,7 +5122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5068,15 +5146,15 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54082569-1F66-4A81-82A5-55EB02F2FDFA}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5134,8 +5212,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5148,14 +5229,10 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="1">
-        <v>40909</v>
-      </c>
-      <c r="N2" s="1">
-        <v>45292</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5168,8 +5245,11 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N3" s="1">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5183,7 +5263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5197,7 +5277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5211,7 +5291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5232,15 +5312,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5298,8 +5378,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5328,7 +5411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5364,15 +5447,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209DCC60-78F8-43ED-886D-BA241054DEC9}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5430,8 +5513,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5472,7 +5558,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5520,15 +5606,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027D9544-C268-4861-A247-C7F1D198DA75}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N3"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5586,8 +5672,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5622,7 +5711,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -5667,15 +5756,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415E4898-F92C-452A-84DB-D5677E1E5900}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="A1:XFD1048576"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5733,8 +5822,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5769,7 +5861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5800,15 +5892,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7E6D6-EE7B-468F-B872-C3BE058F00D0}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="A1:XFD1048576"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5866,8 +5958,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5908,7 +6003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5956,15 +6051,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E2F05C-93A5-44D7-9D90-57CE56FE1A56}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6022,8 +6117,11 @@
       <c r="S1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6061,7 +6159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6102,7 +6200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
All x-axis funs and helpers with some tests
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32DC63B-C0B5-4D47-A238-5EFEF6615979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CA19F0-0D34-42F5-8EFD-176C14611BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="870" yWindow="945" windowWidth="18900" windowHeight="13785" firstSheet="28" activeTab="33" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,18 @@
     <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
     <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
     <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
-    <sheet name="Sheet26" sheetId="26" r:id="rId25"/>
-    <sheet name="Sheet25" sheetId="25" r:id="rId26"/>
+    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
     <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
     <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
     <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
     <sheet name="Sheet30" sheetId="30" r:id="rId30"/>
     <sheet name="Sheet31" sheetId="31" r:id="rId31"/>
     <sheet name="Sheet32" sheetId="32" r:id="rId32"/>
+    <sheet name="Sheet33" sheetId="33" r:id="rId33"/>
+    <sheet name="Sheet34" sheetId="34" r:id="rId34"/>
+    <sheet name="Sheet35" sheetId="35" r:id="rId35"/>
+    <sheet name="Sheet36" sheetId="36" r:id="rId36"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="106">
   <si>
     <t>stacked</t>
   </si>
@@ -367,6 +371,24 @@
   </si>
   <si>
     <t>x_brez_let</t>
+  </si>
+  <si>
+    <t>SURS--1957406S--O--12--M</t>
+  </si>
+  <si>
+    <t>SURS--1957406S--SA--12--M</t>
+  </si>
+  <si>
+    <t>originalni</t>
+  </si>
+  <si>
+    <t>desezonirani</t>
+  </si>
+  <si>
+    <t>indeks (2015 = 100)</t>
+  </si>
+  <si>
+    <t>mio eur</t>
   </si>
 </sst>
 </file>
@@ -723,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80EE0B4-0DE5-4420-9F2D-2330D5CD04DC}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
@@ -2868,7 +2890,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3635,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3781,7 +3803,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3942,11 +3964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4017,73 +4039,11 @@
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="1">
-        <v>36557</v>
-      </c>
-      <c r="N2" s="1">
-        <v>37316</v>
-      </c>
-      <c r="O2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="1">
-        <v>36557</v>
-      </c>
-      <c r="N3" s="1">
-        <v>37316</v>
-      </c>
-      <c r="O3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2">
+        <v>2010</v>
       </c>
     </row>
   </sheetData>
@@ -4092,11 +4052,11 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4167,11 +4127,73 @@
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2">
-        <v>2010</v>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N2" s="1">
+        <v>37316</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>36557</v>
+      </c>
+      <c r="N3" s="1">
+        <v>37316</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4184,7 +4206,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4343,7 +4365,7 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4524,7 +4546,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,7 +4867,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4961,7 +4983,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5149,7 +5171,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5303,6 +5325,464 @@
       </c>
       <c r="E7" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF287603-5FF0-4041-8000-1633844CCF37}">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40179</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAA108-54D8-4A2C-BF68-31C7D1B2946D}">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905DD0A-4072-45DC-A9D1-1BE1A5C155D2}">
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F6706C-2935-4CD2-9CCE-C53CC432F086}">
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>2015</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="P4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add language support and transformation order
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CA19F0-0D34-42F5-8EFD-176C14611BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAE7236-5EFF-412C-B256-79A16127AAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="945" windowWidth="18900" windowHeight="13785" firstSheet="28" activeTab="33" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="109">
   <si>
     <t>stacked</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>mio eur</t>
+  </si>
+  <si>
+    <t>drseca_najprej</t>
+  </si>
+  <si>
+    <t>leva_os_en</t>
+  </si>
+  <si>
+    <t>leva_os_si</t>
   </si>
 </sst>
 </file>
@@ -743,15 +752,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80EE0B4-0DE5-4420-9F2D-2330D5CD04DC}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -812,8 +821,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -828,15 +846,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB519D6D-497D-4A71-AA43-35FF7CBDA7D6}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -897,8 +915,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -942,7 +969,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -987,15 +1014,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C50B29-7A1F-44EC-A2E3-6FFB5D7AF5C3}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1056,8 +1083,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1101,7 +1137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1146,15 +1182,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D794E32-1D66-4AE3-9459-DCC88E8958D7}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1215,8 +1251,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1257,7 +1302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1340,15 +1385,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C3197-EE10-4F45-AA72-93BAA0310B66}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1409,8 +1454,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1451,7 +1505,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1524,7 +1578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1569,15 +1623,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A0D24B-06B1-46C1-B24E-D0229212BA8F}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1638,8 +1692,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1683,7 +1746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1724,7 +1787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1769,15 +1832,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384968AD-14AF-4C49-8E39-1D8EB64036E4}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1838,8 +1901,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1883,7 +1955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +1993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1963,15 +2035,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5A0802-79CF-41E4-9C0C-B7CF9AB66D55}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2032,8 +2104,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2080,7 +2161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2121,7 +2202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2166,15 +2247,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF6D7A-E8BF-4A5F-92E8-83A3842A5065}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2235,8 +2316,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2283,7 +2373,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2324,7 +2414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2369,15 +2459,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A051C55C-5114-4B50-9EEA-9971CA4766EF}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2438,8 +2528,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2483,7 +2582,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +2623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2569,15 +2668,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6814E3-30B1-4C15-9D30-846626E50BDB}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2638,8 +2737,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2686,7 +2794,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2733,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2784,15 +2892,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDA8BA5-AD9E-45CA-A388-27BBF83C10CE}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2853,8 +2961,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2887,15 +3004,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67294519-493C-4162-90F2-F70A28CBB2F0}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2956,8 +3073,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3004,7 +3130,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3045,7 +3171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3086,7 +3212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3133,7 +3259,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3177,7 +3303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -3218,7 +3344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -3266,15 +3392,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C29FF1A-9024-4DF3-916F-A0BDB0709BF3}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3335,8 +3461,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3383,7 +3518,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3424,7 +3559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3465,7 +3600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3510,15 +3645,15 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F90AD-04CA-45FB-9D9A-2BBE8BFC6DB7}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3579,8 +3714,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -3594,7 +3738,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -3608,7 +3752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3632,15 +3776,15 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184719B6-2593-48D2-ACDD-B538913534C8}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3701,8 +3845,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3752,7 +3905,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3800,15 +3953,15 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA275B0-0109-45DF-8346-6D8E9FCBBD4F}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3869,8 +4022,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -3917,7 +4079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3965,15 +4127,15 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4034,8 +4196,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4053,15 +4224,15 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4122,8 +4293,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4158,7 +4338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4203,10 +4383,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6187-8CFA-4331-9ECF-E1D00B50A721}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4214,7 +4394,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4275,8 +4455,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4314,7 +4503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4362,10 +4551,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324E071-F609-4FB8-B88D-8F0EE9A8EC4A}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,7 +4562,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4434,8 +4623,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4473,7 +4671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4514,7 +4712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4525,7 +4723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -4543,10 +4741,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4B2C62-126F-422E-B778-C7A7EC6134D3}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4554,7 +4752,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4615,8 +4813,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4657,7 +4864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -4668,7 +4875,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -4679,7 +4886,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4717,7 +4924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -4735,15 +4942,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A43C6C-A966-4635-89A5-EACCD8BF4906}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4804,8 +5011,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4831,7 +5047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4864,15 +5080,15 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4933,8 +5149,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -4951,7 +5176,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -4962,7 +5187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4980,10 +5205,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C665D4F1-6FFE-4D8B-A6C9-DB93740290E1}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4991,7 +5216,7 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5052,8 +5277,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5076,7 +5310,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5093,7 +5327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5110,7 +5344,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5127,7 +5361,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5144,7 +5378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5168,15 +5402,15 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54082569-1F66-4A81-82A5-55EB02F2FDFA}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5237,8 +5471,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5254,7 +5497,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5271,7 +5514,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5285,7 +5528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5299,7 +5542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5313,7 +5556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5334,15 +5577,15 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF287603-5FF0-4041-8000-1633844CCF37}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5403,8 +5646,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -5418,7 +5670,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -5426,7 +5678,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5441,15 +5693,15 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAA108-54D8-4A2C-BF68-31C7D1B2946D}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5510,8 +5762,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5527,7 +5788,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5543,7 +5804,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5564,15 +5825,15 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905DD0A-4072-45DC-A9D1-1BE1A5C155D2}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5633,8 +5894,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -5648,7 +5918,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -5667,15 +5937,15 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F6706C-2935-4CD2-9CCE-C53CC432F086}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5736,8 +6006,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -5751,7 +6030,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -5763,7 +6042,7 @@
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -5792,15 +6071,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5861,8 +6140,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5891,7 +6179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -5927,15 +6215,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209DCC60-78F8-43ED-886D-BA241054DEC9}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5996,8 +6284,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6038,7 +6335,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6086,15 +6383,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027D9544-C268-4861-A247-C7F1D198DA75}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6155,8 +6452,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6191,7 +6497,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -6236,15 +6542,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415E4898-F92C-452A-84DB-D5677E1E5900}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6305,8 +6611,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6341,7 +6656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6372,15 +6687,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7E6D6-EE7B-468F-B872-C3BE058F00D0}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6441,8 +6756,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6483,7 +6807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6531,15 +6855,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E2F05C-93A5-44D7-9D90-57CE56FE1A56}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="U1" sqref="U1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6600,8 +6924,17 @@
       <c r="T1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6639,7 +6972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6680,7 +7013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Y axis labels with language support
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAE7236-5EFF-412C-B256-79A16127AAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4239D7A8-FA49-4061-9A78-14B49B6DF393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="25" activeTab="32" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="118">
   <si>
     <t>stacked</t>
   </si>
@@ -398,6 +398,33 @@
   </si>
   <si>
     <t>leva_os_si</t>
+  </si>
+  <si>
+    <t>mio_eur</t>
+  </si>
+  <si>
+    <t>desna_os_si</t>
+  </si>
+  <si>
+    <t>desna_os_en</t>
+  </si>
+  <si>
+    <t>legenda_en</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>Lots of euros</t>
+  </si>
+  <si>
+    <t>Ful evrotov</t>
   </si>
 </sst>
 </file>
@@ -752,15 +779,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80EE0B4-0DE5-4420-9F2D-2330D5CD04DC}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -830,8 +857,20 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -846,15 +885,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB519D6D-497D-4A71-AA43-35FF7CBDA7D6}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -924,8 +963,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -969,7 +1017,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1014,15 +1062,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C50B29-7A1F-44EC-A2E3-6FFB5D7AF5C3}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1092,8 +1140,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1137,7 +1194,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1182,15 +1239,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D794E32-1D66-4AE3-9459-DCC88E8958D7}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1260,8 +1317,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1302,7 +1368,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1340,7 +1406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1385,15 +1451,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C3197-EE10-4F45-AA72-93BAA0310B66}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1463,8 +1529,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1505,7 +1580,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1543,7 +1618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1578,7 +1653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1623,15 +1698,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A0D24B-06B1-46C1-B24E-D0229212BA8F}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1701,8 +1776,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1746,7 +1830,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1787,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1832,15 +1916,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384968AD-14AF-4C49-8E39-1D8EB64036E4}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1910,8 +1994,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1955,7 +2048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1993,7 +2086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2035,15 +2128,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5A0802-79CF-41E4-9C0C-B7CF9AB66D55}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2113,8 +2206,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2161,7 +2263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2202,7 +2304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2247,15 +2349,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF6D7A-E8BF-4A5F-92E8-83A3842A5065}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2325,8 +2427,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2373,7 +2484,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2414,7 +2525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2459,15 +2570,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A051C55C-5114-4B50-9EEA-9971CA4766EF}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2537,8 +2648,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2582,7 +2702,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2623,7 +2743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2668,15 +2788,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6814E3-30B1-4C15-9D30-846626E50BDB}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2746,8 +2866,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2794,7 +2923,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2841,7 +2970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2892,15 +3021,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDA8BA5-AD9E-45CA-A388-27BBF83C10CE}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2970,8 +3099,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3004,15 +3142,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67294519-493C-4162-90F2-F70A28CBB2F0}">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3082,8 +3220,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3130,7 +3277,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3171,7 +3318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3212,7 +3359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3259,7 +3406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3303,7 +3450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -3344,7 +3491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -3392,15 +3539,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C29FF1A-9024-4DF3-916F-A0BDB0709BF3}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3470,8 +3617,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3518,7 +3674,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3559,7 +3715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3600,7 +3756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3645,15 +3801,15 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F90AD-04CA-45FB-9D9A-2BBE8BFC6DB7}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3723,8 +3879,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -3738,7 +3903,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -3752,7 +3917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3776,15 +3941,15 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184719B6-2593-48D2-ACDD-B538913534C8}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3854,8 +4019,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3905,7 +4079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3953,15 +4127,15 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA275B0-0109-45DF-8346-6D8E9FCBBD4F}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4031,8 +4205,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -4079,7 +4262,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4127,15 +4310,15 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4205,8 +4388,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4224,15 +4416,15 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4302,8 +4494,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4338,7 +4539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4383,10 +4584,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6187-8CFA-4331-9ECF-E1D00B50A721}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,7 +4595,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4464,8 +4665,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4503,7 +4713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4551,10 +4761,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324E071-F609-4FB8-B88D-8F0EE9A8EC4A}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4562,7 +4772,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4632,8 +4842,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4671,7 +4890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4712,7 +4931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4723,7 +4942,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -4741,10 +4960,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4B2C62-126F-422E-B778-C7A7EC6134D3}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4752,7 +4971,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4822,8 +5041,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4864,7 +5092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -4875,7 +5103,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -4886,7 +5114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4924,7 +5152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -4942,15 +5170,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A43C6C-A966-4635-89A5-EACCD8BF4906}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5020,8 +5248,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5047,7 +5284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5080,15 +5317,15 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5158,8 +5395,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -5176,7 +5422,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -5187,7 +5433,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5205,10 +5451,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C665D4F1-6FFE-4D8B-A6C9-DB93740290E1}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5216,7 +5462,7 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5286,8 +5532,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5310,7 +5565,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5327,7 +5582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5344,7 +5599,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5361,7 +5616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5378,7 +5633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5402,15 +5657,15 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54082569-1F66-4A81-82A5-55EB02F2FDFA}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5480,8 +5735,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5497,7 +5761,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5514,7 +5778,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5528,7 +5792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5542,7 +5806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5556,7 +5820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5577,15 +5841,15 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF287603-5FF0-4041-8000-1633844CCF37}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5655,8 +5919,20 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -5669,21 +5945,36 @@
       <c r="N2" s="1">
         <v>44927</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>117</v>
+      </c>
+      <c r="W2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
       <c r="C3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>85</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -5693,15 +5984,15 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAA108-54D8-4A2C-BF68-31C7D1B2946D}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5771,8 +6062,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5788,7 +6088,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5804,7 +6104,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5825,15 +6125,15 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905DD0A-4072-45DC-A9D1-1BE1A5C155D2}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5903,8 +6203,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -5918,7 +6227,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -5937,15 +6246,15 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F6706C-2935-4CD2-9CCE-C53CC432F086}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6015,8 +6324,20 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -6030,7 +6351,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -6042,7 +6363,7 @@
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -6071,15 +6392,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6149,8 +6470,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6179,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6215,15 +6545,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209DCC60-78F8-43ED-886D-BA241054DEC9}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6293,8 +6623,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6335,7 +6674,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6383,15 +6722,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027D9544-C268-4861-A247-C7F1D198DA75}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6461,8 +6800,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6497,7 +6845,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -6542,15 +6890,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415E4898-F92C-452A-84DB-D5677E1E5900}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6620,8 +6968,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6656,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6687,15 +7044,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7E6D6-EE7B-468F-B872-C3BE058F00D0}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6765,8 +7122,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6807,7 +7173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6855,15 +7221,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E2F05C-93A5-44D7-9D90-57CE56FE1A56}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:W1"/>
+      <selection activeCell="X1" sqref="X1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6933,8 +7299,17 @@
       <c r="W1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6972,7 +7347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7013,7 +7388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Fix failing tests, add output to pdf fun
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/pub_test_df.xlsx
+++ b/tests/testthat/testdata/pub_test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARvisualisR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4239D7A8-FA49-4061-9A78-14B49B6DF393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258D2A6F-572A-4EE4-9A0E-33CAE3AF9E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="25" activeTab="32" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2" xr2:uid="{39A53309-B5C2-4694-BD56-2AC72C43F4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="118">
   <si>
     <t>stacked</t>
   </si>
@@ -781,6 +781,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80EE0B4-0DE5-4420-9F2D-2330D5CD04DC}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB519D6D-497D-4A71-AA43-35FF7CBDA7D6}">
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
@@ -877,109 +983,6 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB519D6D-497D-4A71-AA43-35FF7CBDA7D6}">
-  <dimension ref="A1:Z3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>99</v>
-      </c>
-      <c r="U1" t="s">
-        <v>106</v>
-      </c>
-      <c r="V1" t="s">
-        <v>108</v>
-      </c>
-      <c r="W1" t="s">
-        <v>107</v>
-      </c>
-      <c r="X1" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1062,15 +1065,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C50B29-7A1F-44EC-A2E3-6FFB5D7AF5C3}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1149,8 +1152,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1239,15 +1245,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D794E32-1D66-4AE3-9459-DCC88E8958D7}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1326,8 +1332,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1368,7 +1377,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1451,15 +1460,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C3197-EE10-4F45-AA72-93BAA0310B66}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1538,8 +1547,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1653,7 +1665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1698,15 +1710,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A0D24B-06B1-46C1-B24E-D0229212BA8F}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1785,8 +1797,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1830,7 +1845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1871,7 +1886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1916,15 +1931,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384968AD-14AF-4C49-8E39-1D8EB64036E4}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2003,8 +2018,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2048,7 +2066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2086,7 +2104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2128,15 +2146,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5A0802-79CF-41E4-9C0C-B7CF9AB66D55}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2215,8 +2233,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2263,7 +2284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2304,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2349,15 +2370,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FF6D7A-E8BF-4A5F-92E8-83A3842A5065}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2436,8 +2457,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2484,7 +2508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2525,7 +2549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2570,15 +2594,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A051C55C-5114-4B50-9EEA-9971CA4766EF}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2657,8 +2681,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2702,7 +2729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2743,7 +2770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2788,15 +2815,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6814E3-30B1-4C15-9D30-846626E50BDB}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2875,8 +2902,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2923,7 +2953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2970,7 +3000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3021,15 +3051,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDA8BA5-AD9E-45CA-A388-27BBF83C10CE}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3108,8 +3138,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3142,15 +3175,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67294519-493C-4162-90F2-F70A28CBB2F0}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3229,8 +3262,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3277,7 +3313,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3318,7 +3354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3359,7 +3395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3406,7 +3442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3450,7 +3486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -3491,7 +3527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -3539,15 +3575,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C29FF1A-9024-4DF3-916F-A0BDB0709BF3}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3626,8 +3662,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3674,7 +3713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3715,7 +3754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3756,7 +3795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3801,15 +3840,15 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0F90AD-04CA-45FB-9D9A-2BBE8BFC6DB7}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3888,8 +3927,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -3903,7 +3945,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -3917,7 +3959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3941,15 +3983,15 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184719B6-2593-48D2-ACDD-B538913534C8}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4028,8 +4070,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4079,7 +4124,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4127,15 +4172,15 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA275B0-0109-45DF-8346-6D8E9FCBBD4F}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4214,8 +4259,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -4262,7 +4310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4310,15 +4358,15 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F21370-6104-4EA9-9387-90FAA3EFC6A2}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4397,8 +4445,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4416,15 +4467,15 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB58369-401F-4EA0-A11B-4F4C68AB6743}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4503,8 +4554,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4539,7 +4593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4584,10 +4638,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6187-8CFA-4331-9ECF-E1D00B50A721}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4595,7 +4649,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4674,8 +4728,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4713,7 +4770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4761,10 +4818,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324E071-F609-4FB8-B88D-8F0EE9A8EC4A}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4772,7 +4829,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4851,8 +4908,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -4890,7 +4950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -4931,7 +4991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4942,7 +5002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -4960,10 +5020,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4B2C62-126F-422E-B778-C7A7EC6134D3}">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4971,7 +5031,7 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5050,8 +5110,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -5092,7 +5155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -5103,7 +5166,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -5114,7 +5177,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -5152,7 +5215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -5170,15 +5233,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A43C6C-A966-4635-89A5-EACCD8BF4906}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5257,8 +5320,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5284,7 +5350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5317,15 +5383,15 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C45945-4AE3-406B-B043-F2A523A19530}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5404,8 +5470,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -5422,7 +5491,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -5433,7 +5502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5451,10 +5520,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C665D4F1-6FFE-4D8B-A6C9-DB93740290E1}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5462,7 +5531,7 @@
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5541,8 +5610,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5565,7 +5637,7 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5582,7 +5654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5599,7 +5671,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5616,7 +5688,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5633,7 +5705,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5657,15 +5729,15 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54082569-1F66-4A81-82A5-55EB02F2FDFA}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5744,8 +5816,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -5761,7 +5836,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -5778,7 +5853,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -5792,7 +5867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -5806,7 +5881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -5820,7 +5895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -5843,8 +5918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF287603-5FF0-4041-8000-1633844CCF37}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5984,15 +6059,15 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAA108-54D8-4A2C-BF68-31C7D1B2946D}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6071,8 +6146,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -6088,7 +6166,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -6104,7 +6182,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -6125,15 +6203,15 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8905DD0A-4072-45DC-A9D1-1BE1A5C155D2}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6212,8 +6290,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -6227,7 +6308,7 @@
         <v>40179</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -6248,7 +6329,153 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F6706C-2935-4CD2-9CCE-C53CC432F086}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U1" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="1">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>2015</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="P4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
@@ -6339,149 +6566,6 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
-      </c>
-      <c r="M2" s="1">
-        <v>40179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>2015</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="P4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC052CEB-AD24-4388-B9F9-889BDD482904}">
-  <dimension ref="A1:Z3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>99</v>
-      </c>
-      <c r="U1" t="s">
-        <v>106</v>
-      </c>
-      <c r="V1" t="s">
-        <v>108</v>
-      </c>
-      <c r="W1" t="s">
-        <v>107</v>
-      </c>
-      <c r="X1" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -6509,7 +6593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6545,15 +6629,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209DCC60-78F8-43ED-886D-BA241054DEC9}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6632,8 +6716,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6674,7 +6761,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -6722,15 +6809,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027D9544-C268-4861-A247-C7F1D198DA75}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6809,8 +6896,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -6845,7 +6935,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -6890,15 +6980,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415E4898-F92C-452A-84DB-D5677E1E5900}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6977,8 +7067,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7013,7 +7106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -7044,15 +7137,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7E6D6-EE7B-468F-B872-C3BE058F00D0}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -7131,8 +7224,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7173,7 +7269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7221,15 +7317,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E2F05C-93A5-44D7-9D90-57CE56FE1A56}">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:Z1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -7308,8 +7404,11 @@
       <c r="Z1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7347,7 +7446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7388,7 +7487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>